<commit_message>
four-panel population figure and insect trend update complete
</commit_message>
<xml_diff>
--- a/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_3282.xlsx
+++ b/fourth_pass/welfare_results/3282/analysis_results/cor_and_elas_3282.xlsx
@@ -1528,33 +1528,47 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="n">
+        <v>-0.99949039209519</v>
+      </c>
       <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
+        <v>-167966135.730231</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.95662930260746</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.999490392095189</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.95662930260746</v>
+      </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>123411.461836652</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>7054577.7006697</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
+        <v>-2938368.1389679</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.956629302607457</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.999490392095189</v>
+      </c>
+      <c r="L24" t="n">
+        <v>-0.95662930260746</v>
+      </c>
       <c r="M24" t="n">
-        <v>0.000000000000501440558108759</v>
+        <v>50.2489665458678</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0000000000367305357094737</v>
+        <v>2872.38505727593</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>-2938368.1389679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>